<commit_message>
remove year from GDPpc column
</commit_message>
<xml_diff>
--- a/2025/website/website_data_partitions.xlsx
+++ b/2025/website/website_data_partitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishka_sharma/Desktop/AQLI/REPO/annual.updates/2025/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B291E-EBD1-3F41-B750-696E951B02DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6889F46-54CE-174E-BDFD-CD5C8ADCE128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="36980" windowHeight="26760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21760" yWindow="500" windowWidth="36980" windowHeight="26760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Percentage of countries with open data</t>
   </si>
   <si>
-    <t>GDP per capita (2023)</t>
-  </si>
-  <si>
     <t>pm1998</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>Upper middle income</t>
+  </si>
+  <si>
+    <t>GDP per capita</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:CA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CA2" sqref="CA2:CA12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -688,7 +688,7 @@
   <sheetData>
     <row r="1" spans="1:79" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -697,240 +697,240 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>18.52</v>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
         <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>81</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4">
         <v>92.31</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="5" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5">
         <v>57.14</v>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>36.840000000000003</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7">
         <v>7.41</v>
@@ -2361,10 +2361,10 @@
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <v>75</v>
@@ -2600,10 +2600,10 @@
     </row>
     <row r="9" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>81.819999999999993</v>
@@ -2839,10 +2839,10 @@
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11">
         <v>88.24</v>
@@ -3317,10 +3317,10 @@
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13">
         <v>34.619999999999997</v>
@@ -3795,10 +3795,10 @@
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
         <v>92</v>
-      </c>
-      <c r="B14" t="s">
-        <v>93</v>
       </c>
       <c r="C14">
         <v>97.3</v>
@@ -4034,10 +4034,10 @@
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15">
         <v>66.27</v>
@@ -4273,10 +4273,10 @@
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>95</v>
-      </c>
-      <c r="B16" t="s">
-        <v>96</v>
       </c>
       <c r="C16">
         <v>11.54</v>
@@ -4512,10 +4512,10 @@
     </row>
     <row r="17" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17">
         <v>45.1</v>
@@ -4751,10 +4751,10 @@
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18">
         <v>50</v>

</xml_diff>